<commit_message>
Loads correct board, displays everything correctly
</commit_message>
<xml_diff>
--- a/ClueBoard Test Locations.xlsx
+++ b/ClueBoard Test Locations.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="-180" windowWidth="17235" windowHeight="6150"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16215" windowHeight="8325"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Macro1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H26"/>
 </workbook>
 </file>
 
@@ -656,11 +658,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="CA12" sqref="CA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,7 +3006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
@@ -5087,7 +5101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>